<commit_message>
einiges an arbeit an der arbeit
</commit_message>
<xml_diff>
--- a/simulation_dp_serov/test_EKF/Qmin.xlsx
+++ b/simulation_dp_serov/test_EKF/Qmin.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -19,18 +19,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Anregung</t>
   </si>
   <si>
     <t>Regelung</t>
   </si>
+  <si>
+    <t>Aussc hwing?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -334,7 +337,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -342,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D11"/>
+      <selection activeCell="A15" sqref="A15:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +475,69 @@
         <v>10</v>
       </c>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.01</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>